<commit_message>
Casos de prueba , Floyd, Dijkstra, rutas
Casos de prueba terminados
Floyd y Dijkstra modificados
Solución grafo desconectado
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\ED Proyecto #2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IC-2001-II-2-P-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabla pivote" sheetId="5" r:id="rId1"/>
-    <sheet name="Veneno Game - Casos" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabla pivote" sheetId="6" r:id="rId1"/>
+    <sheet name="Aeropuertos - Casos" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Certificado">'Veneno Game - Casos'!$G$4:$G$6</definedName>
-    <definedName name="Estado">'Veneno Game - Casos'!$G$4:$G$6</definedName>
+    <definedName name="Certificado">'Aeropuertos - Casos'!$G$4:$G$6</definedName>
+    <definedName name="Estado">'Aeropuertos - Casos'!$G$4:$G$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>Casos de prueba</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Pendiente</t>
   </si>
   <si>
-    <t>Al iniciar el juego se abre correctamente el socket.</t>
-  </si>
-  <si>
     <t>Se ejecute background en un proceso de Windows.</t>
   </si>
   <si>
@@ -103,36 +100,18 @@
     <t>La animacion se ejecuta correctamente y la persona puede interactuar con el mouse</t>
   </si>
   <si>
-    <t>Presionar el boton de Calcular ruta</t>
-  </si>
-  <si>
     <t>Se valida que el manual de usuario se pueda desplegar</t>
   </si>
   <si>
     <t>La animacion del manual de usuario se puede desplegar de manera correcta.</t>
   </si>
   <si>
-    <t>Valiacion al precional el botono calcular inicie el mapa</t>
-  </si>
-  <si>
-    <t>Inicializacion del mapa con las rutas</t>
-  </si>
-  <si>
     <t>El mapa carga las rutas iniciales</t>
   </si>
   <si>
     <t>Despliegue del nombre de aeropuerto</t>
   </si>
   <si>
-    <t>Se puede visualizar el nombre del aeropuerto en cada vertice</t>
-  </si>
-  <si>
-    <t>Depliegue de la imagen al precional el aeropuerto</t>
-  </si>
-  <si>
-    <t>Se valida el despligue de la imagen con el nombre correcto al precionar un vertice.</t>
-  </si>
-  <si>
     <t>Todos los aeropuertos conectados</t>
   </si>
   <si>
@@ -142,42 +121,9 @@
     <t>Se puede escoger el aeropuerto de destino y origen</t>
   </si>
   <si>
-    <t>Se valida que despliegua la lista de aeropuertos de forma correcta</t>
-  </si>
-  <si>
-    <t>Se puede escoger el algoritmo al cual aplicar al mapa</t>
-  </si>
-  <si>
-    <t>Puede escogerse el algoritmo del aeropuerto correspondiente</t>
-  </si>
-  <si>
-    <t>El boton de calcular envia los datos al socket</t>
-  </si>
-  <si>
-    <t>Cuando se pulsa el boton de calcular se envian los datos de origen destino y algoritmo.</t>
-  </si>
-  <si>
-    <t>El algortimo disktra retorna la ruta optima</t>
-  </si>
-  <si>
-    <t>El algortimo floyd retorna la ruta optima</t>
-  </si>
-  <si>
-    <t>El algortimo wharsall retorna el archivo esperado</t>
-  </si>
-  <si>
     <t>El algortimo kruskal retorna el archivo esperado</t>
   </si>
   <si>
-    <t>Se retorna la ruta mas optima con este algoritmo</t>
-  </si>
-  <si>
-    <t>Se escribe el archivo, con el algoritmo de wharsall</t>
-  </si>
-  <si>
-    <t>Se escribe el archivo, con el algoritmo de kruskal</t>
-  </si>
-  <si>
     <t>Se dibuja en el mapa la ruta esperada</t>
   </si>
   <si>
@@ -196,58 +142,202 @@
     <t>Se permite al usuario escoger la ruta para guardar el archivo</t>
   </si>
   <si>
-    <t>La opcion de descarga permite abrir el manual de usuario en una nueva pestaña</t>
-  </si>
-  <si>
     <t>Se abre una nueva pestaña con el manual de usuario</t>
   </si>
   <si>
-    <t>Se dibuja una animacion de avion al calcular ruta</t>
-  </si>
-  <si>
-    <t>El avion se mueve paulatinamente al calcular una ruta</t>
-  </si>
-  <si>
-    <t>Al precional el boton de comprar</t>
-  </si>
-  <si>
-    <t>Cuando se preciona el boton de comprar se simula la compra</t>
-  </si>
-  <si>
     <t>Se despliega la ruta con escalas y sin escalas</t>
   </si>
   <si>
-    <t>Mediante una animacion se muestra la ruta sin escalas</t>
-  </si>
-  <si>
-    <t>Se despliega el precio correcto pasando por los nodos</t>
-  </si>
-  <si>
-    <t>Despliega el precio calculada la ruta de la forma correcta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se puede calcular mas de una ruta dentro de la misma ventana </t>
-  </si>
-  <si>
     <t>Se le permite al usuario poder calcular otras rutas en otros aeropuertos.</t>
   </si>
   <si>
-    <t>Los aeropuertos se encuentran geograficamente correctos</t>
-  </si>
-  <si>
     <t>Las posiciones son precisas dentro del mapa</t>
   </si>
   <si>
-    <t>Se permite acercarse o alejarse del mapa para poder ver los nodos</t>
-  </si>
-  <si>
-    <t>Se pude ver con  facilidad los nodos y permite realizar un zoom</t>
-  </si>
-  <si>
-    <t>Al iniciar el juego el sistema carga los aeropuertos desde el archivo</t>
-  </si>
-  <si>
-    <t>Al iniciar el juego el sistema carga las rutas desde el archivo</t>
+    <t>Al iniciar se ejecutable como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En todas las pantallas de juego existe un enlace de atrás validando en los casos en los que no pueda ir, como al iniciar la consola de juego. </t>
+  </si>
+  <si>
+    <t>Enlaces de atrás correctamente validados a las pantallas correspondientes</t>
+  </si>
+  <si>
+    <t>Presionar el botón de Calcular ruta</t>
+  </si>
+  <si>
+    <t>Validacion al presionar el botón calcular inicie el mapa</t>
+  </si>
+  <si>
+    <t>Inicialización del mapa con las rutas</t>
+  </si>
+  <si>
+    <t>Se puede visualizar el nombre del aeropuerto en cada vértice</t>
+  </si>
+  <si>
+    <t>Despliegue de la imagen al presionar el aeropuerto</t>
+  </si>
+  <si>
+    <t>Se valida el despligue de la imagen con el nombre correcto al presionar un vértice.</t>
+  </si>
+  <si>
+    <t>Se valida que despliega la lista de aeropuertos de forma correcta</t>
+  </si>
+  <si>
+    <t>Se puede escoger el algoritmo con el cual encontrar la ruta más corta</t>
+  </si>
+  <si>
+    <t>Se puede escoger entre Dijkstra y Floyd</t>
+  </si>
+  <si>
+    <t>El botón de calcular envía los datos al socket</t>
+  </si>
+  <si>
+    <t>Cuando se pulsa el botón de calcular se envían los datos de origen, destino y algoritmo.</t>
+  </si>
+  <si>
+    <t>Se retorna la ruta más corta con este algoritmo</t>
+  </si>
+  <si>
+    <t>El algoritmo de Dijkstra retorna la ruta más corta</t>
+  </si>
+  <si>
+    <t>El algoritmo de Floyd retorna la ruta más corta</t>
+  </si>
+  <si>
+    <t>La opción de descarga permite abrir el manual de usuario en una nueva pestaña</t>
+  </si>
+  <si>
+    <t>Se dibuja una animación del avión al calcular ruta</t>
+  </si>
+  <si>
+    <t>El avión se mueve del aeropuerto de origen al de destino.</t>
+  </si>
+  <si>
+    <t>Al presionar el botón de comprar</t>
+  </si>
+  <si>
+    <t>Cuando se presiona el botón de comprar se simula la compra</t>
+  </si>
+  <si>
+    <t>El algoritmo Warshall retorna el archivo esperado</t>
+  </si>
+  <si>
+    <t>La ruta que se despliega concuerda con la etiqueta, ya sea con o sin escalas</t>
+  </si>
+  <si>
+    <t>Se despliega el precio correcto de la ruta a tomar</t>
+  </si>
+  <si>
+    <t>Despliega el precio calculando la ruta de la forma correcta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se puede calcular más de una ruta dentro de la misma ventana </t>
+  </si>
+  <si>
+    <t>Los aeropuertos se encuentran colocados de una manera geográficamente correcta</t>
+  </si>
+  <si>
+    <t>Se permite acercarse o alejarse del mapa para poder ver los aeropuertos</t>
+  </si>
+  <si>
+    <t>Se escribe el archivo, con el algoritmo de Warshall</t>
+  </si>
+  <si>
+    <t>Se escribe el archivo, con el algoritmo de Kruskal</t>
+  </si>
+  <si>
+    <t>Se puede ver con  facilidad los aeropuertos y permite realizar un zoom</t>
+  </si>
+  <si>
+    <t>Las información de los aeropuertos es cargada desde un archivo de texto</t>
+  </si>
+  <si>
+    <t>Al iniciar el juego el sistema carga los aeropuertos desde el archivo en la interfaz gráfica</t>
+  </si>
+  <si>
+    <t>Al iniciar el juego el sistema carga los aeropuertos desde el archivo en la lógica C++</t>
+  </si>
+  <si>
+    <t>Al iniciar el juego el sistema carga las rutas desde el archivo en la interfaz gráfica</t>
+  </si>
+  <si>
+    <t>Al iniciar el juego el sistema carga las rutas desde el archivo en la lógica C++</t>
+  </si>
+  <si>
+    <t>Las información de las rutas es cargada desde un archivo de texto</t>
+  </si>
+  <si>
+    <t>Al iniciar el juego del gato se abre correctamente el socket.</t>
+  </si>
+  <si>
+    <t>Al iniciar el simulador se abre correctamente el socket.</t>
+  </si>
+  <si>
+    <t>Iniciar el simulador</t>
+  </si>
+  <si>
+    <t>Se le asigna un nombre al jugador</t>
+  </si>
+  <si>
+    <t>El nombre se le asigna correctamente y es con el que se le llama durante todo el juego</t>
+  </si>
+  <si>
+    <t>Al presionar el botón terminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El juego termina la partida</t>
+  </si>
+  <si>
+    <t>Opciones para jugar de primero o segundo</t>
+  </si>
+  <si>
+    <t>Determinan el orden del juego a partir de esa decisión del usuario</t>
+  </si>
+  <si>
+    <t>Nueva partida</t>
+  </si>
+  <si>
+    <t>Crea una nueva partida del juego</t>
+  </si>
+  <si>
+    <t>Las jugadas de la computadora solo nos dejan empatar o perder</t>
+  </si>
+  <si>
+    <t>Al jugar contra la computadora</t>
+  </si>
+  <si>
+    <t>Al realizar movimientos erróneos</t>
+  </si>
+  <si>
+    <t>El juego da una retroalimentación indicando que la jugada es incorrecta</t>
+  </si>
+  <si>
+    <t>El árbol minmax se crea correctamente</t>
+  </si>
+  <si>
+    <t>Se crea un árbol con sus nodos en tiempo real y dandole siempre ventaja a la compuatdora</t>
+  </si>
+  <si>
+    <t>Se utilizan estructuras propias</t>
+  </si>
+  <si>
+    <t>Para crear el árbol se utilizan TDA propias como las vistas en clases</t>
+  </si>
+  <si>
+    <t>Para crear los grafo y los algoritmos se utilizan TDA propias como las vistas en clases</t>
+  </si>
+  <si>
+    <t>Las imágenes se enlazan correctamente</t>
+  </si>
+  <si>
+    <t>Se muestra la imagen de cada aeropuerto de manera correcta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se puede llegar desde cualquier aeropuerto a cualquier otro. </t>
+  </si>
+  <si>
+    <t>El grafo es conectado</t>
   </si>
 </sst>
 </file>
@@ -318,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,10 +431,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -352,21 +445,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -400,6 +478,21 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -414,7 +507,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="José Ceciliano" refreshedDate="42844.981260763889" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="admin" refreshedDate="42889.90272233796" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
@@ -426,7 +519,7 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Resultado esperado" numFmtId="0">
-      <sharedItems longText="1"/>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Estado" numFmtId="0">
       <sharedItems count="2">
@@ -447,20 +540,20 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
   <r>
     <n v="1"/>
-    <s v="Al iniciar el juego se abre correctamente el socket."/>
+    <s v="Al iniciar el simulador se abre correctamente el socket."/>
     <s v="Se ejecute background en un proceso de Windows."/>
     <x v="0"/>
   </r>
   <r>
     <n v="2"/>
     <s v="Al presionar el ejecutable se ejecuta el apache y las dependencias."/>
-    <s v="Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
+    <s v="Al iniciar se ejecutable como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
     <x v="0"/>
   </r>
   <r>
     <n v="3"/>
-    <s v="Iniciar el juego."/>
-    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal."/>
+    <s v="Iniciar el simulador"/>
+    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia el juego principal."/>
     <x v="0"/>
   </r>
   <r>
@@ -471,285 +564,285 @@
   </r>
   <r>
     <n v="5"/>
+    <s v="En todas las pantallas de juego existe un enlace de atrás validando en los casos en los que no pueda ir, como al iniciar la consola de juego. "/>
+    <s v="Enlaces de atrás correctamente validados a las pantallas correspondientes"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="Animacion del juego inicial"/>
+    <s v="La animacion se ejecuta correctamente y la persona puede interactuar con el mouse"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="Se valida que el manual de usuario se pueda desplegar"/>
+    <s v="La animacion del manual de usuario se puede desplegar de manera correcta."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="Presionar el botón de Calcular ruta"/>
+    <s v="Validacion al presionar el botón calcular inicie el mapa"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="Inicialización del mapa con las rutas"/>
+    <s v="El mapa carga las rutas iniciales"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="Despliegue del nombre de aeropuerto"/>
+    <s v="Se puede visualizar el nombre del aeropuerto en cada vértice"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="Despliegue de la imagen al presionar el aeropuerto"/>
+    <s v="Se valida el despligue de la imagen con el nombre correcto al presionar un vértice."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="Todos los aeropuertos conectados"/>
+    <s v="Existe por lo menos un camino para llegar al aeropuerto correspondiente"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="Se puede escoger el aeropuerto de destino y origen"/>
+    <s v="Se valida que despliega la lista de aeropuertos de forma correcta"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="Se puede escoger el algoritmo con el cual encontrar la ruta más corta"/>
+    <s v="Se puede escoger entre Dijkstra y Floyd"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <s v="El botón de calcular envía los datos al socket"/>
+    <s v="Cuando se pulsa el botón de calcular se envían los datos de origen, destino y algoritmo."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <s v="El algoritmo de Dijkstra retorna la ruta más corta"/>
+    <s v="Se retorna la ruta más corta con este algoritmo"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="El algoritmo de Floyd retorna la ruta más corta"/>
+    <s v="Se retorna la ruta más corta con este algoritmo"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="El algoritmo Warshall retorna el archivo esperado"/>
+    <s v="Se escribe el archivo, con el algoritmo de Warshall"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="El algortimo kruskal retorna el archivo esperado"/>
+    <s v="Se escribe el archivo, con el algoritmo de Kruskal"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="Se dibuja en el mapa la ruta esperada"/>
+    <s v="Se dibuja en el mapa la ruta esperada del retorno del algoritmo"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="El boton de descarga permite guardar el archivo"/>
+    <s v="Al precional descargas me permite escoger el algoritmo"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="Al descargar el archivo permite escoger la ruta"/>
+    <s v="Se permite al usuario escoger la ruta para guardar el archivo"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="La opción de descarga permite abrir el manual de usuario en una nueva pestaña"/>
+    <s v="Se abre una nueva pestaña con el manual de usuario"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="Se dibuja una animación del avión al calcular ruta"/>
+    <s v="El avión se mueve del aeropuerto de origen al de destino."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="Al presionar el botón de comprar"/>
+    <s v="Cuando se presiona el botón de comprar se simula la compra"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Se despliega la ruta con escalas y sin escalas"/>
+    <s v="La ruta que se despliega concuerda con la etiqueta, ya sea con o sin escalas"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="Se despliega el precio correcto de la ruta a tomar"/>
+    <s v="Despliega el precio calculando la ruta de la forma correcta"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Se puede calcular más de una ruta dentro de la misma ventana "/>
+    <s v="Se le permite al usuario poder calcular otras rutas en otros aeropuertos."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Los aeropuertos se encuentran colocados de una manera geográficamente correcta"/>
+    <s v="Las posiciones son precisas dentro del mapa"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Se permite acercarse o alejarse del mapa para poder ver los aeropuertos"/>
+    <s v="Se puede ver con  facilidad los aeropuertos y permite realizar un zoom"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Al iniciar el juego el sistema carga los aeropuertos desde el archivo en la interfaz gráfica"/>
+    <s v="Las información de los aeropuertos es cargada desde un archivo de texto"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Al iniciar el juego el sistema carga los aeropuertos desde el archivo en la lógica C++"/>
+    <s v="Las información de los aeropuertos es cargada desde un archivo de texto"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Al iniciar el juego el sistema carga las rutas desde el archivo en la interfaz gráfica"/>
+    <s v="Las información de las rutas es cargada desde un archivo de texto"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="Al iniciar el juego el sistema carga las rutas desde el archivo en la lógica C++"/>
+    <s v="Las información de las rutas es cargada desde un archivo de texto"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Se utilizan estructuras propias"/>
+    <s v="Para crear los grafo y los algoritmos se utilizan TDA propias como las vistas en clases"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Las imágenes se enlazan correctamente"/>
+    <s v="Se muestra la imagen de cada aeropuerto de manera correcta"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="El grafo es conectado"/>
+    <s v="Se puede llegar desde cualquier aeropuerto a cualquier otro. "/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Se utilizan estructuras propias"/>
+    <s v="Para crear el árbol se utilizan TDA propias como las vistas en clases"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="El árbol minmax se crea correctamente"/>
+    <s v="Se crea un árbol con sus nodos en tiempo real y dandole siempre ventaja a la compuatdora"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Al realizar movimientos erróneos"/>
+    <s v="El juego da una retroalimentación indicando que la jugada es incorrecta"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Al jugar contra la computadora"/>
+    <s v="Las jugadas de la computadora solo nos dejan empatar o perder"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Nueva partida"/>
+    <s v="Crea una nueva partida del juego"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Opciones para jugar de primero o segundo"/>
+    <s v="Determinan el orden del juego a partir de esa decisión del usuario"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Al presionar el botón terminar"/>
+    <s v=" El juego termina la partida"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Al iniciar el juego del gato se abre correctamente el socket."/>
+    <s v="Se ejecute background en un proceso de Windows."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Al presionar el ejecutable se ejecuta el apache y las dependencias."/>
+    <s v="Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <s v="Iniciar el juego."/>
+    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia el juego principal."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Se le asigna un nombre al jugador"/>
+    <s v="El nombre se le asigna correctamente y es con el que se le llama durante todo el juego"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="49"/>
     <s v="En todas las pantallas de juego existe un enlace a atrás validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
     <s v="Enlaces de atrás correctamente validados alas pantallas correspondientes"/>
     <x v="0"/>
   </r>
   <r>
-    <n v="6"/>
-    <s v="Movimientos &quot;drag and drop&quot; del juego."/>
-    <s v="La animación del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <s v="Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero"/>
-    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no está en el caldero correcto. "/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="Presionar el boton de juego."/>
-    <s v="Se valida la activación y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="9"/>
-    <s v="Asignar la cantidad de jugadores en uno."/>
-    <s v="No se puede crear solo un jugador, el mínimo son dos."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="10"/>
-    <s v="Asignar la cantidad de jugadores en dos."/>
-    <s v="La cantidad es aceptada correctamente."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="11"/>
-    <s v="Asignar la cantidad de jugadores en siete."/>
-    <s v="No es posible, el máximo son seis jugadores."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="12"/>
-    <s v="No digita el nombre del jugador al crearlo."/>
-    <s v="El sistema no permite continuar sin un nombre."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="13"/>
-    <s v="Digita un nombre al jugador al crearlo."/>
-    <s v="Se le asigna el string digitado como nombre al guardar el jugador en la lista."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="14"/>
-    <s v="Se crean seis jugadores, se les asigna un nombre a cada uno."/>
-    <s v="La lista de jugadores debe contener 6 jugadores, cada uno con el nombre asignado, y un id que indica el orden en que fueron creados."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="15"/>
-    <s v="Busca un jugador según su posición en la lista (la posición existe)."/>
-    <s v="La lista devuelve el objeto jugador en esa posición (desde modo consola)."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="16"/>
-    <s v="Busca un jugador según su posición en la lista (la posición no existe)."/>
-    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía (desde modo consola)."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="17"/>
-    <s v="Busca la baraja de cartas en mano de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas en mano, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="18"/>
-    <s v="Busca la baraja de cartas  comidas de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas comidas, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="19"/>
-    <s v="Busca la baraja de cartas veneno de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas veneno, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="20"/>
-    <s v="Llama a la opción barajar antes de empezar la ronda."/>
-    <s v="Se reparte una cantidad de cartas cada jugador según la cantidad de jugadores activos, estas cartas son repartidas de manera aleatoria."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="21"/>
-    <s v="Después de barajar  se consulta el pozo para repartir."/>
-    <s v="Devuelve el pozo, este debe ser el pozo original, menos las cartas previamente repartidas."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="22"/>
-    <s v="Llama a la opción barajar, mientras algún jugador todavía tiene cartas."/>
-    <s v="Sólo se puede barajar cuando todos los jugadores no tengan ninguna carta en la mano."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="23"/>
-    <s v="Llama a la opción barajar (en el pozo no quedan suficientes cartas para repartir según las reglas)"/>
-    <s v="Se termina la ronda."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="24"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero vacío."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="25"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero no vacío, pero que tiene la misma nomenclatura. El total del caldero es menor que trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="26"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero con diferente nomenclatura."/>
-    <s v="El sistema rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="27"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero. El total del caldero da más de trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="28"/>
-    <s v="Se añade una carta veneno a un caldero no vacío. El total del caldero es menor que trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="29"/>
-    <s v="Se añade una carta veneno a un caldero vacío. El jugador tiene más cartas en la mano."/>
-    <s v="Se rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="30"/>
-    <s v="Se añade una carta veneno a un caldero vacío. El jugador sólo tiene esa carta en la mano."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="31"/>
-    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador sólo tiene esa carta en la mano."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="32"/>
-    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador tiene más cartas en la mano."/>
-    <s v="El sistema rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="33"/>
-    <s v="Se añade una carta veneno a un caldero. El total del caldero da más de trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="34"/>
-    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador tiene cartas en la mano."/>
-    <s v="El sistema no permite continuar con el juego hasta que el jugador en el turno mueva la carta."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="35"/>
-    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas."/>
-    <s v="Todos los jugadores se quedan sin cartas al mismo tiempo."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="36"/>
-    <s v="Llama a ver ronda en medio del juego."/>
-    <s v="Se muestran los resultados hasta ese momento de cada jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="37"/>
-    <s v="Se termina una ronda."/>
-    <s v="Muestra una pantalla con los resultados de la ronda."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="38"/>
-    <s v="Se come un caldero que contiene venenos."/>
-    <s v="Se añaden estas cartas venenos a la del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="39"/>
-    <s v="Al ejecutar el juego se abra automáticamente el socket."/>
-    <s v="Se abre el socket y despliega el menú del juego."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="40"/>
-    <s v="Llamar la función undo, en medio de una ronda."/>
-    <s v="Devuelve al movimiento anterior."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="41"/>
-    <s v="Llamar la función redo, sin haber realizado un undo."/>
-    <s v="No se podruce ningún cambio."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="42"/>
-    <s v="Llamar la función redo, después de un undo."/>
-    <s v="Vuelve a hacer el movimiento que el undo quitó."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="43"/>
-    <s v="Llamar la función reset al empezar una ronda."/>
-    <s v="No se realiza ningún cambio."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="44"/>
-    <s v="Llamar la función reset en medio de una ronda."/>
-    <s v="Devuelve la ronda al principio"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="45"/>
-    <s v="Mientras se ejecuta una acción en el servidor no se modifque la interfaz."/>
-    <s v="Muestra en pantalla un ícono que indica que se está cargando."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="46"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno."/>
-    <s v="Se acaba la ronda y dicho jugador sale del juego."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="47"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Ningún jugador tiene cartas veneno."/>
-    <s v="Se acaba el juego."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="48"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Todos los jugadores tienen la misma cantidad de cartas venenos."/>
-    <s v="Se acaba el juego."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="49"/>
-    <s v="Se acaban las cartas en el pozo para repartir. Varios jugadores tienen la misma cantidad de venenos."/>
-    <s v="Se crea una neva ronda, y se sacan del juego los jugadores que tengan menor cantidad de venenos."/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="50"/>
-    <s v="Se acaban las cartas en el pozo para repartir. Sólo quedan dos jugadores."/>
-    <s v="Se saca el jugador con menos cartas venenos, el otro es el perdedor."/>
+    <s v="Animacion del juego inicial"/>
+    <s v="La animacion se ejecuta correctamente y la persona puede interactuar con el mouse"/>
     <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -796,13 +889,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B4:E54"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id " dataDxfId="3"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="2"/>
-    <tableColumn id="3" name="Resultado esperado" dataDxfId="1"/>
-    <tableColumn id="4" name="Estado" dataDxfId="0"/>
+    <tableColumn id="1" name="Id " dataDxfId="6"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="3" name="Resultado esperado" dataDxfId="4"/>
+    <tableColumn id="4" name="Estado" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1107,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,10 +1212,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,12 +1231,12 @@
         <v>6</v>
       </c>
       <c r="B5" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8">
         <v>50</v>
@@ -1158,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,12 +1265,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -1206,10 +1299,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
@@ -1223,10 +1316,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
@@ -1240,10 +1333,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>5</v>
@@ -1255,10 +1348,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>5</v>
@@ -1269,10 +1362,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>5</v>
@@ -1283,10 +1376,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>5</v>
@@ -1297,10 +1390,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>5</v>
@@ -1311,10 +1404,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>5</v>
@@ -1325,10 +1418,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>5</v>
@@ -1339,24 +1432,24 @@
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>5</v>
@@ -1367,10 +1460,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>5</v>
@@ -1381,10 +1474,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>5</v>
@@ -1395,24 +1488,24 @@
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>5</v>
@@ -1423,10 +1516,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>5</v>
@@ -1437,10 +1530,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>5</v>
@@ -1451,10 +1544,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>5</v>
@@ -1465,13 +1558,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1479,10 +1572,10 @@
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>5</v>
@@ -1493,10 +1586,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>5</v>
@@ -1507,10 +1600,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>5</v>
@@ -1521,10 +1614,10 @@
         <v>23</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>5</v>
@@ -1535,10 +1628,10 @@
         <v>24</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>5</v>
@@ -1549,10 +1642,10 @@
         <v>25</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>5</v>
@@ -1563,10 +1656,10 @@
         <v>26</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>5</v>
@@ -1577,24 +1670,24 @@
         <v>27</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>28</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>5</v>
@@ -1605,10 +1698,10 @@
         <v>29</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>5</v>
@@ -1622,7 +1715,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>5</v>
@@ -1633,11 +1726,13 @@
         <v>31</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="E35" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1645,213 +1740,263 @@
         <v>32</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="11">
+      <c r="B37" s="12">
         <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="12">
+        <v>34</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
+        <v>35</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="12">
+        <v>36</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="12">
+        <v>37</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="10">
+        <v>38</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="10">
+        <v>39</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="10">
+        <v>40</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="10">
+        <v>41</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="10">
+        <v>42</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="10">
+        <v>43</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="10">
+        <v>44</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="10">
+        <v>45</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="11">
-        <v>34</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="E49" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="10">
+        <v>46</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="10">
+        <v>47</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="11">
-        <v>35</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="D51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="10">
+        <v>48</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="10">
+        <v>49</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="10">
+        <v>50</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="11">
-        <v>36</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="11">
-        <v>37</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="11">
-        <v>38</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="11">
-        <v>39</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="11">
-        <v>40</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="11">
-        <v>41</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="11">
-        <v>42</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="11">
-        <v>43</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="11">
-        <v>44</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="11">
-        <v>45</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="11">
-        <v>46</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="11">
-        <v>47</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="11">
-        <v>48</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="11">
-        <v>49</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="11">
-        <v>50</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
       <c r="E54" s="3" t="s">
         <v>5</v>
       </c>
@@ -1865,13 +2010,13 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:E54">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Con error">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con error">
       <formula>NOT(ISERROR(SEARCH("Con error",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Pendiente">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendiente">
       <formula>NOT(ISERROR(SEARCH("Pendiente",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Certificado">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Certificado">
       <formula>NOT(ISERROR(SEARCH("Certificado",E5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cambios generales al mapa
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IC-2001-II-2-P-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla pivote" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -408,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,17 +434,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -477,21 +498,6 @@
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -842,7 +848,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -889,13 +895,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B4:E54"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id " dataDxfId="6"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="5"/>
-    <tableColumn id="3" name="Resultado esperado" dataDxfId="4"/>
-    <tableColumn id="4" name="Estado" dataDxfId="3"/>
+    <tableColumn id="1" name="Id " dataDxfId="3"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="2"/>
+    <tableColumn id="3" name="Resultado esperado" dataDxfId="1"/>
+    <tableColumn id="4" name="Estado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1200,7 +1206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1251,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,12 +1271,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -1750,7 +1756,7 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="12">
+      <c r="B37" s="11">
         <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1764,7 +1770,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <v>34</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1778,7 +1784,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>35</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1792,7 +1798,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="12">
+      <c r="B40" s="11">
         <v>36</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -1806,7 +1812,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="12">
+      <c r="B41" s="11">
         <v>37</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -1823,13 +1829,13 @@
       <c r="B42" s="10">
         <v>38</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1837,13 +1843,13 @@
       <c r="B43" s="10">
         <v>39</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1851,13 +1857,13 @@
       <c r="B44" s="10">
         <v>40</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1865,13 +1871,13 @@
       <c r="B45" s="10">
         <v>41</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1879,13 +1885,13 @@
       <c r="B46" s="10">
         <v>42</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1893,13 +1899,13 @@
       <c r="B47" s="10">
         <v>43</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1907,13 +1913,13 @@
       <c r="B48" s="10">
         <v>44</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1921,13 +1927,13 @@
       <c r="B49" s="10">
         <v>45</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1935,13 +1941,13 @@
       <c r="B50" s="10">
         <v>46</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1949,13 +1955,13 @@
       <c r="B51" s="10">
         <v>47</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1963,13 +1969,13 @@
       <c r="B52" s="10">
         <v>48</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1977,13 +1983,13 @@
       <c r="B53" s="10">
         <v>49</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1991,13 +1997,13 @@
       <c r="B54" s="10">
         <v>50</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2010,13 +2016,13 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:E54">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con error">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Con error">
       <formula>NOT(ISERROR(SEARCH("Con error",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendiente">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Pendiente">
       <formula>NOT(ISERROR(SEARCH("Pendiente",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Certificado">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Certificado">
       <formula>NOT(ISERROR(SEARCH("Certificado",E5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>